<commit_message>
improve test capability, enable checking of sub-entity fields
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBFC899-BB59-4860-975C-30B4653569CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E8C70F-D1E6-4653-9548-7F6AE730C8AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,10 +124,10 @@
     <t>{Project(cond:"{status:{_eq:\"online\"},Lease_Group:{lease_type:{_eq:\"2\"}}}",order:"") {business_mgr business_unit charge_frequency city province district credit_amount detail_address discount_ratio expire_date guarantee_type id no status name risk_mgr rent_type}}</t>
   </si>
   <si>
-    <t>{Site(cond:"{id:{_eq:\"P000000666\"}}",order:"") { id location commissioning_date state power_station Has_Device_Inverter{ site pr production name type full_generation_hours} }}</t>
-  </si>
-  <si>
     <t>{Project(cond:"{status:{_eq:\"online\"},Lease_Group:{lease_type:{_eq:\"2\"}}}",order:"") {business_mgr business_unit charge_frequency city province district class_level classification_level credit_amount detail_address discount_ratio expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture no status name risk_mgr rent_type invert_Customer(cond:"",order:"") { actual_controller category cid city cname contact contact_detail ctype district enterprise_size group holding_type id is_connected_tx is_gov_fin_customer is_group_customer legal_person_id legal_person major_class middle_class office_address project province registered_address small_class} Restricted_By_Contract(cond:"",order:"") {accumulated_amount charge_frequency contract_amount customer grant_loan_frequency id lease_balance lease_end_time lease_num lease_start_time lease_unit leasing_principal make_loan_day overdue_amount overdue_days overdue_interest overdue_principal payment_method project} Refer_To_Lease_Group(cond:"",order:"") {asset_type count discount_ratio id lease_net_val lease_type lease_type_gb lease_type_yj nominal_cost project transfer_price unit_price}} }</t>
+  </si>
+  <si>
+    <t>{Site(cond:"{id:{_eq:\"P000000666\"}}",order:"") { id location commissioning_date state power_station Has_Device_Inverter   { site pr production name type full_generation_hours} }}</t>
   </si>
 </sst>
 </file>
@@ -917,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3">
         <v>200</v>
@@ -935,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3">
         <v>200</v>

</xml_diff>

<commit_message>
add complex condition checking function
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z0044p8f\Downloads\test-data-xls\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407E96C7-11BB-4769-90DA-70055B40AF27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9941565F-D2FD-4A57-BE8F-89B4F431E6F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -85,15 +85,6 @@
   </si>
   <si>
     <t>[Project][business_mgr,risk_mgr,rent_type][{charge_frequency: {_eq: 2}}]</t>
-  </si>
-  <si>
-    <t>[Project][business_mgr,risk_mgr,rent_type][{charge_frequency: {_neq: 2}}]</t>
-  </si>
-  <si>
-    <t>[Project][business_mgr,risk_mgr,rent_type][{charge_frequency: {_in: [2, 3]}}][][]</t>
-  </si>
-  <si>
-    <t>[Project][business_mgr,risk_mgr,rent_type][{charge_frequency: {_nin: [2, 3]}}][][]</t>
   </si>
   <si>
     <t>[Project][][][no asc][1,10]</t>
@@ -1003,6 +994,15 @@
   </si>
   <si>
     <t>expectJson</t>
+  </si>
+  <si>
+    <t>[Project][business_mgr,risk_mgr,rent_type,charge_frequency][{charge_frequency: {_neq: 2}}]</t>
+  </si>
+  <si>
+    <t>[Project][business_mgr,risk_mgr,rent_type,charge_frequency][{charge_frequency: {_in: [2, 3]}}][][]</t>
+  </si>
+  <si>
+    <t>[Project][business_mgr,risk_mgr,rent_type,charge_frequency][{charge_frequency: {_nin: [2, 3]}}][][]</t>
   </si>
 </sst>
 </file>
@@ -1368,17 +1368,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="1"/>
-    <col min="4" max="4" width="36.6640625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="12.6640625" style="1"/>
+    <col min="1" max="2" width="30.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6328125" style="1"/>
+    <col min="4" max="4" width="36.6328125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="12.6328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1502,7 +1502,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>15</v>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>15</v>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>15</v>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>15</v>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>15</v>
@@ -1616,16 +1616,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.6640625" style="6" customWidth="1"/>
-    <col min="4" max="6" width="12.6640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="2" width="30.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.6328125" style="6" customWidth="1"/>
+    <col min="4" max="6" width="12.6328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -1681,7 +1681,7 @@
         <v>101301</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1690,7 +1690,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3">
         <v>200</v>
@@ -1708,7 +1708,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>200</v>
@@ -1726,7 +1726,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3">
         <v>200</v>
@@ -1735,7 +1735,7 @@
         <v>101302</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1744,7 +1744,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3">
         <v>200</v>
@@ -1762,7 +1762,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3">
         <v>200</v>
@@ -1780,7 +1780,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D9" s="3">
         <v>200</v>
@@ -1798,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3">
         <v>200</v>
@@ -1816,7 +1816,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D11" s="3">
         <v>200</v>
@@ -1843,12 +1843,12 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.6640625" style="1" customWidth="1"/>
-    <col min="3" max="7" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="30.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.6328125" style="1" customWidth="1"/>
+    <col min="3" max="7" width="12.6328125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1865,59 +1865,59 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="C2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="3">
-        <v>100000</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="F2" s="3">
         <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="208" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="220.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="3">
-        <v>100000</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1934,12 +1934,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.6640625" style="1" customWidth="1"/>
-    <col min="3" max="7" width="12.6640625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.77734375" style="1"/>
+    <col min="1" max="1" width="30.6328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.6328125" style="1" customWidth="1"/>
+    <col min="3" max="7" width="12.6328125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1956,21 +1956,21 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="3">
         <v>100000</v>
@@ -1979,21 +1979,21 @@
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C3" s="3">
         <v>100000</v>
@@ -2002,21 +2002,21 @@
         <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:7" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3">
         <v>100000</v>
@@ -2025,13 +2025,13 @@
         <v>9</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F4" s="3">
         <v>1</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor improve, handle the situation when return data is null
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9941565F-D2FD-4A57-BE8F-89B4F431E6F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D76078D-DE34-46E2-9847-E94FF0741558}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="58">
   <si>
     <t>description</t>
   </si>
@@ -1003,6 +1003,10 @@
   </si>
   <si>
     <t>[Project][business_mgr,risk_mgr,rent_type,charge_frequency][{charge_frequency: {_nin: [2, 3]}}][][]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Contract(cond:"{project:{_eq:33}}",order:"") { accumulated_amount charge_frequency contract_amount customer grant_loan_frequency id lease_balance lease_end_time lease_num lease_start_time lease_unit leasing_principal make_loan_day overdue_amount overdue_days overdue_interest overdue_principal payment_method project invert_Project(cond:"",order:"") { business_mgr business_unit charge_frequency city province district class_level classification_level credit_amount detail_address discount_ratio expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture no status name risk_mgr rent_type Refer_To_Lease_Group(cond:"",order:"") { asset_type count discount_ratio id lease_net_val lease_type lease_type_gb lease_type_yj nominal_cost project transfer_price unit_price Refer_To_Power_Station_Properties(cond:"",order:"") { ps_type structure avg_annual_eq_hours capacity } }  } invert_Customer(cond:"",order:"") { actual_controller category cid city cname contact contact_detail ctype district enterprise_size group holding_type id is_connected_tx is_gov_fin_customer is_group_customer legal_person_id legal_person major_class middle_class office_address project province registered_address small_class } } }
+    </t>
   </si>
 </sst>
 </file>
@@ -1368,7 +1372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
@@ -1614,10 +1618,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1649,12 +1653,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3">
         <v>200</v>
@@ -1667,30 +1673,34 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D3" s="3">
         <v>200</v>
       </c>
       <c r="E3" s="3">
-        <v>101301</v>
+        <v>100000</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>22</v>
+      <c r="C4" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="D4" s="3">
         <v>200</v>
@@ -1708,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3">
         <v>200</v>
@@ -1723,19 +1733,19 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3">
         <v>200</v>
       </c>
       <c r="E6" s="3">
-        <v>101302</v>
+        <v>101301</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1743,8 +1753,8 @@
       <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>26</v>
+      <c r="C7" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D7" s="3">
         <v>200</v>
@@ -1761,8 +1771,8 @@
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>27</v>
+      <c r="C8" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="D8" s="3">
         <v>200</v>
@@ -1777,19 +1787,19 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3">
         <v>200</v>
       </c>
       <c r="E9" s="3">
-        <v>100000</v>
+        <v>101302</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1797,8 +1807,8 @@
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>29</v>
+      <c r="C10" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D10" s="3">
         <v>200</v>
@@ -1815,8 +1825,8 @@
       <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>30</v>
+      <c r="C11" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D11" s="3">
         <v>200</v>
@@ -1825,6 +1835,24 @@
         <v>100000</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3">
+        <v>200</v>
+      </c>
+      <c r="E12" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Jinzu test case complete
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B133E97C-6F12-457A-99EA-996C87ABF97E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432514E9-F6B8-4FF8-A761-3AABB2BE7742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="116">
   <si>
     <t>description</t>
   </si>
@@ -231,6 +231,150 @@
   </si>
   <si>
     <t>{Project(cond:"{status:{_eq:\"online\"}, classification_level:{_eq:\"正常\"}}",order:"") {invert_Customer{cname invalid_field} id status}}</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var1</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{charge_frequency:{_eq:3}}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var2</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{is_manufacture_buy_back:{_eq:false}}",order:"") {business_mgr business_unit charge_frequency city class_level discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{business_mgr:{_eq:\"胡晓峰\"}}",order:"") {business_mgr business_unit charge_frequency city class_level manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{charge_frequency:{_neq:3}}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type}}</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var4</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var5</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{is_manufacture_buy_back:{_neq:false}}",order:"") {business_mgr business_unit charge_frequency city class_level discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var6</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{status:{_neq:\"online\"}}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{business_mgr:{_neq:\"胡晓峰\"}}",order:"") {business_mgr business_unit charge_frequency city class_level manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{charge_frequency:{_gte:3}}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{status: {_gte: \"b\"}}") {business_mgr business_unit charge_frequency city province district credit_amount detail_address discount_ratio expire_date guarantee_type id no status name risk_mgr rent_type}}</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var7</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var8</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var9</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var10</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{charge_frequency:{_gt:3}}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{status: {_gt: \"b\"}}") {business_mgr business_unit charge_frequency city province district credit_amount detail_address discount_ratio expire_date guarantee_type id no status name risk_mgr rent_type}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{charge_frequency:{_lte:3}}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{status: {_lte: \"b\"}}") {business_mgr business_unit charge_frequency city province district credit_amount detail_address discount_ratio expire_date guarantee_type id no status name risk_mgr rent_type}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{charge_frequency:{_lt:3}}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var11</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var12</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var13</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var14</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var15</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var16</t>
+  </si>
+  <si>
+    <t>{Project (cond:"{charge_frequency:{_in:[1,2,3]}}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>{Project (cond:"{charge_frequency:{_nin:[1,2,3]}}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var17</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var18</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var19</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var20</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var21</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var22</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{status: {_lt: \"b\"}}") {business_mgr business_unit charge_frequency city province district credit_amount detail_address discount_ratio expire_date guarantee_type id no status name risk_mgr rent_type}}</t>
+  </si>
+  <si>
+    <t>{Project (cond:"{_and: [{business_mgr:{_in:[\"潘云晖\",\"臧佳宝\" ]}},{status:{_in:[\"archived\" ]}}]}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var23</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var24</t>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-Test-7-var25</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{status:{_in:[\"online\",\"archived\"]}}",order:"") {business_mgr business_unit charge_frequency city province district credit_amount detail_address discount_ratio expire_date guarantee_type id no status name risk_mgr rent_type}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{business_mgr:{_in:[\"潘云晖\",\"臧佳宝\"]}}",order:"") {business_mgr business_unit charge_frequency city province district credit_amount detail_address discount_ratio expire_date guarantee_type id no status name risk_mgr rent_type}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{status:{_nin:[\"online\",\"bbbb\"]}}",order:"") {business_mgr business_unit charge_frequency city province district credit_amount detail_address discount_ratio expire_date guarantee_type id no status name risk_mgr rent_type}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{business_mgr:{_nin:[\"潘云晖\",\"臧佳宝\"]}}",order:"") {business_mgr business_unit charge_frequency city province district credit_amount detail_address discount_ratio expire_date guarantee_type id no status name risk_mgr rent_type}}</t>
+  </si>
+  <si>
+    <t>{Project (cond:"{_or: [{business_mgr:{_in:[\"潘云晖\",\"臧佳宝\"]}},{status:{_in:[\"archived\" ]}}]}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status}}</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{_or: [{business_mgr:{_in:[\"潘云晖\",\"臧佳宝\" ]}},{status:{_in:[\"archived\" ]}}]}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status  invert_Customer (cond:"{id:{_eq:24}}",order:"") {actual_controller category cid city cname contact contact_detail ctype district enterprise_size group holding_type id is_connected_tx is_gov_fin_customer is_group_customer legal_person legal_person_id major_class middle_class office_address project province registered_address small_class}}}</t>
   </si>
 </sst>
 </file>
@@ -887,16 +1031,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="30.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="90.7109375" style="6" customWidth="1"/>
     <col min="4" max="6" width="12.5703125" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
@@ -1261,6 +1405,486 @@
         <v>66</v>
       </c>
     </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="3">
+        <v>200</v>
+      </c>
+      <c r="E19" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="3">
+        <v>200</v>
+      </c>
+      <c r="E20" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="3">
+        <v>200</v>
+      </c>
+      <c r="E21" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="3">
+        <v>200</v>
+      </c>
+      <c r="E22" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="3">
+        <v>200</v>
+      </c>
+      <c r="E23" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="3">
+        <v>200</v>
+      </c>
+      <c r="E24" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="3">
+        <v>200</v>
+      </c>
+      <c r="E25" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="3">
+        <v>200</v>
+      </c>
+      <c r="E26" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="3">
+        <v>200</v>
+      </c>
+      <c r="E27" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="3">
+        <v>200</v>
+      </c>
+      <c r="E28" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="3">
+        <v>200</v>
+      </c>
+      <c r="E29" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="3">
+        <v>200</v>
+      </c>
+      <c r="E30" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="3">
+        <v>200</v>
+      </c>
+      <c r="E31" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="3">
+        <v>200</v>
+      </c>
+      <c r="E32" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="3">
+        <v>200</v>
+      </c>
+      <c r="E33" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="3">
+        <v>200</v>
+      </c>
+      <c r="E34" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="3">
+        <v>200</v>
+      </c>
+      <c r="E35" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="3">
+        <v>200</v>
+      </c>
+      <c r="E36" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D37" s="3">
+        <v>200</v>
+      </c>
+      <c r="E37" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="3">
+        <v>200</v>
+      </c>
+      <c r="E38" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="3">
+        <v>200</v>
+      </c>
+      <c r="E39" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" s="3">
+        <v>200</v>
+      </c>
+      <c r="E40" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D41" s="3">
+        <v>200</v>
+      </c>
+      <c r="E41" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="3">
+        <v>200</v>
+      </c>
+      <c r="E42" s="3">
+        <v>100000</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add jinzu user query test
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432514E9-F6B8-4FF8-A761-3AABB2BE7742}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153031D7-FC93-4481-A206-3DA244C3EADC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
     <sheet name="getDataGraphQL" sheetId="3" r:id="rId2"/>
+    <sheet name="getLeaseDetails" sheetId="4" r:id="rId3"/>
+    <sheet name="getLeaseList" sheetId="5" r:id="rId4"/>
+    <sheet name="getProjectDetails" sheetId="6" r:id="rId5"/>
+    <sheet name="getProjectByCondition" sheetId="8" r:id="rId6"/>
+    <sheet name="getSiteDetails" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="133">
   <si>
     <t>description</t>
   </si>
@@ -375,6 +380,455 @@
   </si>
   <si>
     <t>{Project(cond:"{_or: [{business_mgr:{_in:[\"潘云晖\",\"臧佳宝\" ]}},{status:{_in:[\"archived\" ]}}]}",order:"") {business_mgr business_unit charge_frequency city class_level classification_level credit_amount detail_address discount_ratio district expire_date guarantee_type id is_manufacture_buy_back is_manufacture_leasing manufacture name no province rent_type risk_mgr status  invert_Customer (cond:"{id:{_eq:24}}",order:"") {actual_controller category cid city cname contact contact_detail ctype district enterprise_size group holding_type id is_connected_tx is_gov_fin_customer is_group_customer legal_person legal_person_id major_class middle_class office_address project province registered_address small_class}}}</t>
+  </si>
+  <si>
+    <t>jasonTemplate</t>
+  </si>
+  <si>
+    <t>查看某个租赁物的详细信息</t>
+  </si>
+  <si>
+    <t>queryString</t>
+  </si>
+  <si>
+    <t>{Lease(cond:"{id:{_eq:667}}", order:"") {
+	lease_type_gb
+	lending
+	lposition
+	invoice_no
+	project
+	lease_type_yj
+	brand_name
+	unit_price
+	serial_num
+	discount_ratio
+	transfer_price
+	lease_net_val
+	nominal_cost
+	supplier
+	asset_type
+	name
+	lease_type
+	position
+	id
+	purchase_time
+	status
+	lease_group
+	product_model
+	invert_Lease_Group( cond:"", order:"") {
+		lease_net_val
+		transfer_price
+		lease_type_gb
+		nominal_cost
+		count
+		asset_type
+		project
+		lease_type_yj
+		id
+		lease_type
+		unit_price
+		discount_ratio
+		invert_Project( cond:"", order:"") {
+			no
+			rent_type
+			is_manufacture_buy_back
+			classification_level
+			city
+			detail_address
+			charge_frequency
+			credit_amount
+			risk_mgr
+			is_manufacture_leasing
+			business_unit
+			discount_ratio
+			class_level
+			manufacture
+			business_mgr
+			expire_date
+			province
+			district
+			name
+			guarantee_type
+			id
+			status
+			invert_Customer( cond:"", order:"") {
+				registered_address
+				city
+				major_class
+				cname
+				enterprise_size
+				project
+				is_connected_tx
+				legal_person_id
+				small_class
+				province
+				is_gov_fin_customer
+				contact
+				id
+				group
+				legal_person
+				contact_detail
+				actual_controller
+				office_address
+				ctype
+				district
+				is_group_customer
+				middle_class
+				category
+				cid
+				holding_type
+			}
+		}
+		Refer_To_Power_Station_Properties( cond:"", order:"") {
+			avg_annual_eq_hours
+			lease_group
+			ps_type
+			structure
+			capacity
+		}
+	}
+	Refer_To_Power_Station( cond:"", order:"") {
+		id
+		Compose_Of_Site( cond:"", order:"") 
+		{
+			avg_annual_eq_hours
+			avg_irradiance
+			capacity
+			city
+			commissioning_date
+			grid_inject_production
+			id
+			irradiance
+			location
+			name
+			power_station
+			state
+			sys_engaged_date
+			type
+			voltage_degree
+			Generate_Site_Report( cond:"{report_time:{_eq:\"1582128000000\"}}", order:"") {
+				energy_loss
+				pr
+				peak_power_moment
+				production
+				purchasing_energy
+				sunshin_duration
+				full_generation_hours
+				comprehensive_plant_power_consumption
+				peak_power
+				self_consumed_percent
+				site
+				revenue
+				report_time
+				comprehensive_plant_power_consumption_rate
+				self_consumed_production
+				energy_loss_rate
+				equivalent_hours
+				pr_validity
+			}
+			invert_Weather( cond:"", order:"") {
+				max_temperature
+				update_time
+				site
+				rainfall
+				main_weather_station
+				avg_temperature
+				description
+				min_temperature
+			}
+			Involve_Device_Alarm_Event( cond:"", order:"") {
+				alarm_location
+				update_time
+				site
+				alarm_handle_status
+				alarm_template
+				occurring_time
+				event_name
+				id
+				update_by
+				device
+				confirm_time
+			}
+		}
+	}
+}
+}</t>
+  </si>
+  <si>
+    <t>JasonModelSchemaForLeaseDetails.JSON</t>
+  </si>
+  <si>
+    <t>JasonModelSchemaForLeaseList.JSON</t>
+  </si>
+  <si>
+    <t>{Lease(cond:"{project:{_eq:99}}", order:"") {
+	lease_type_gb
+	lending
+	lposition
+	invoice_no
+	project
+	lease_type_yj
+	brand_name
+	unit_price
+	serial_num
+	discount_ratio
+	transfer_price
+	lease_net_val
+	nominal_cost
+	supplier
+	asset_type
+	name
+	lease_type
+	position
+	id
+	purchase_time
+	status
+	lease_group
+	product_model
+	Refer_To_Power_Station(cond:"", order:"") {
+		id
+		Compose_Of_Site(cond:"", order:"") {
+			avg_annual_eq_hours
+			avg_irradiance
+			capacity
+			city
+			commissioning_date
+			grid_inject_production
+			id
+			irradiance
+			location
+			name
+			power_station
+			state
+			sys_engaged_date
+			type
+			voltage_degree
+		}
+	}
+}}</t>
+  </si>
+  <si>
+    <t>根据project id获取租赁物信息列表</t>
+  </si>
+  <si>
+    <t>获取指定项目的详细信息</t>
+  </si>
+  <si>
+    <t>JasonModelSchemaForProjectDetails.JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Contract(cond:"{project:{_eq:99}}", order:"") {
+	accumulated_amount
+	charge_frequency
+	contract_amount
+	customer
+	grant_loan_frequency
+	id
+	lease_balance
+	lease_end_time
+	lease_num
+	lease_start_time
+	lease_unit
+	leasing_principal
+	make_loan_day
+	overdue_amount
+	overdue_days
+	overdue_interest
+	overdue_principal
+	payment_method
+	project
+	invert_Project(cond:"", order:"") {
+		business_mgr
+		business_unit
+		charge_frequency
+		city
+		province
+		district
+		class_level
+		classification_level
+		credit_amount
+		detail_address
+		discount_ratio
+		expire_date
+		guarantee_type
+		id
+		is_manufacture_buy_back
+		is_manufacture_leasing
+		manufacture
+		no
+		status
+		name
+		risk_mgr
+		rent_type
+		Refer_To_Lease_Group(cond:"", order:"") {
+			asset_type
+			count
+			discount_ratio
+			id
+			lease_net_val
+			lease_type
+			lease_type_gb
+			lease_type_yj
+			nominal_cost
+			project
+			transfer_price
+			unit_price
+			Refer_To_Power_Station_Properties(cond:"", order:"") {
+				ps_type
+				structure
+				avg_annual_eq_hours
+				capacity
+			}
+		}
+	}
+	invert_Customer(cond:"", order:"") {
+		actual_controller
+		category
+		cid
+		city
+		cname
+		contact
+		contact_detail
+		ctype
+		district
+		enterprise_size
+		group
+		holding_type
+		id
+		is_connected_tx
+		is_gov_fin_customer
+		is_group_customer
+		legal_person_id
+		legal_person
+		major_class
+		middle_class
+		office_address
+		project
+		province
+		registered_address
+		small_class
+	}
+}}
+</t>
+  </si>
+  <si>
+    <t>通过项目类型对项目进行过滤</t>
+  </si>
+  <si>
+    <t>JasonModelSchemaForGetProjectByCondition.JSON</t>
+  </si>
+  <si>
+    <t>查看电站的逆变器信息</t>
+  </si>
+  <si>
+    <t>{Site(cond:"{id:{_eq:\"P000000666\"}}",order:"") {
+	id
+	location
+	commissioning_date
+	state
+	power_station
+	Has_Device_Inverter {
+		site
+		pr
+		production
+		name
+		type
+		full_generation_hours
+	}
+}}</t>
+  </si>
+  <si>
+    <t>JasonModelSchemaForSiteDetails.JSON</t>
+  </si>
+  <si>
+    <t>{Project(cond:"{status:{_eq:\"online\"},Lease_Group:{lease_type:{_eq:\"2\"}}}",order:"") {
+	business_mgr
+	business_unit
+	charge_frequency
+	city
+	province
+	district
+	class_level
+	classification_level
+	credit_amount
+	detail_address
+	discount_ratio
+	expire_date
+	guarantee_type
+	id
+	is_manufacture_buy_back
+	is_manufacture_leasing
+	manufacture
+	no
+	status
+	name
+	risk_mgr
+	rent_type
+	invert_Customer(cond:"",order:"") {
+		actual_controller
+		category
+		cid
+		city
+		cname
+		contact
+		contact_detail
+		ctype
+		district
+		enterprise_size
+		group
+		holding_type
+		id
+		is_connected_tx
+		is_gov_fin_customer
+		is_group_customer
+		legal_person_id
+		legal_person
+		major_class
+		middle_class
+		office_address
+		project
+		province
+		registered_address
+		small_class
+	}
+	Restricted_By_Contract(cond:"",order:"")
+	{
+	  accumulated_amount
+	  charge_frequency
+	  contract_amount
+	  customer
+	  grant_loan_frequency
+	  id
+	  lease_balance
+	  lease_end_time
+	  lease_num
+	  lease_start_time
+	  lease_unit
+	  leasing_principal
+	  make_loan_day
+	  overdue_amount
+	  overdue_days
+	  overdue_interest
+	  overdue_principal
+	  payment_method
+	  project
+	}
+	Refer_To_Lease_Group(cond:"",order:"")
+	{
+	  asset_type
+	  count
+	  discount_ratio
+	  id
+	  lease_net_val
+	  lease_type
+	  lease_type_gb
+	  lease_type_yj
+	  nominal_cost
+	  project
+	  transfer_price
+	  unit_price
+	}
+}}</t>
   </si>
 </sst>
 </file>
@@ -739,18 +1193,18 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="1"/>
-    <col min="4" max="4" width="36.5703125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="12.5703125" style="1"/>
+    <col min="1" max="2" width="30.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" style="1"/>
+    <col min="4" max="4" width="36.54296875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="12.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -776,7 +1230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -798,7 +1252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
@@ -822,7 +1276,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -846,7 +1300,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -868,7 +1322,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -890,7 +1344,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -912,7 +1366,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>1</v>
@@ -934,7 +1388,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
@@ -956,7 +1410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>1</v>
@@ -978,7 +1432,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>1</v>
@@ -1000,7 +1454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>1</v>
@@ -1033,19 +1487,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D13" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="90.7109375" style="6" customWidth="1"/>
-    <col min="4" max="6" width="12.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="2" width="30.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="90.7265625" style="6" customWidth="1"/>
+    <col min="4" max="6" width="12.54296875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1065,7 +1519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -1085,7 +1539,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
@@ -1105,7 +1559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -1125,7 +1579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -1145,7 +1599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
@@ -1165,7 +1619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
@@ -1185,7 +1639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>48</v>
       </c>
@@ -1205,7 +1659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -1225,7 +1679,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
@@ -1245,7 +1699,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
@@ -1265,7 +1719,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>55</v>
       </c>
@@ -1285,7 +1739,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1305,7 +1759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>61</v>
       </c>
@@ -1325,7 +1779,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>62</v>
       </c>
@@ -1345,7 +1799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>62</v>
       </c>
@@ -1365,7 +1819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>63</v>
       </c>
@@ -1385,7 +1839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>64</v>
       </c>
@@ -1405,7 +1859,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>68</v>
       </c>
@@ -1425,7 +1879,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>70</v>
       </c>
@@ -1445,7 +1899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>74</v>
       </c>
@@ -1465,7 +1919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
@@ -1485,7 +1939,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>77</v>
       </c>
@@ -1505,7 +1959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>82</v>
       </c>
@@ -1525,7 +1979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>83</v>
       </c>
@@ -1545,7 +1999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>84</v>
       </c>
@@ -1565,7 +2019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>85</v>
       </c>
@@ -1585,7 +2039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>91</v>
       </c>
@@ -1605,7 +2059,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>92</v>
       </c>
@@ -1625,7 +2079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>93</v>
       </c>
@@ -1645,7 +2099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>94</v>
       </c>
@@ -1665,7 +2119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>95</v>
       </c>
@@ -1685,7 +2139,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>96</v>
       </c>
@@ -1705,7 +2159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>99</v>
       </c>
@@ -1725,7 +2179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>100</v>
       </c>
@@ -1745,7 +2199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>101</v>
       </c>
@@ -1765,7 +2219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>102</v>
       </c>
@@ -1785,7 +2239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>103</v>
       </c>
@@ -1805,7 +2259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>104</v>
       </c>
@@ -1825,7 +2279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>107</v>
       </c>
@@ -1845,7 +2299,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>108</v>
       </c>
@@ -1865,7 +2319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>109</v>
       </c>
@@ -1890,4 +2344,344 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52831BC6-0353-44A5-AF16-53FEEB981D2D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" customWidth="1"/>
+    <col min="3" max="3" width="40.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="6" max="7" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5016205C-392A-4756-BA1F-C46FE02BB072}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" customWidth="1"/>
+    <col min="3" max="3" width="40.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="6" max="7" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00996915-EEF2-4680-8A3C-4155BADE3794}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" customWidth="1"/>
+    <col min="3" max="3" width="40.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="6" max="7" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FACB25C-715F-46EA-8323-1EF68080F322}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" customWidth="1"/>
+    <col min="3" max="3" width="40.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="6" max="7" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A553E58-7867-4004-A3CD-42B74E09076D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="30.6328125" customWidth="1"/>
+    <col min="3" max="3" width="40.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
+    <col min="6" max="7" width="12.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="3">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add test case of AppClientAuthenticationForK8sTests
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E960E6CC-5948-44DC-898B-0E74E03DDA37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE17ED6-9DF2-4CCE-8E23-75A0EF6EF44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="getProjectDetails" sheetId="6" r:id="rId5"/>
     <sheet name="getProjectByCondition" sheetId="8" r:id="rId6"/>
     <sheet name="getSiteDetails" sheetId="9" r:id="rId7"/>
+    <sheet name="getSchemaWithAuth" sheetId="10" r:id="rId8"/>
+    <sheet name="getAllCacheStatsWithAuth" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="154">
   <si>
     <t>description</t>
   </si>
@@ -827,6 +829,69 @@
 	}
 }}</t>
   </si>
+  <si>
+    <t>clientId</t>
+  </si>
+  <si>
+    <t>clientSecret</t>
+  </si>
+  <si>
+    <t>grantType</t>
+  </si>
+  <si>
+    <t>accessTokenUrl</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>1c481daa-c881-4ab6-803a-f3808ebd2548</t>
+  </si>
+  <si>
+    <t>Client Credentials</t>
+  </si>
+  <si>
+    <t>http://140.231.89.106:30701/auth/realms/Test/protocol/openid-connect/token</t>
+  </si>
+  <si>
+    <t>JinZu-App client authentication-Test-1</t>
+  </si>
+  <si>
+    <t>JinZu-App client authentication-Test-2</t>
+  </si>
+  <si>
+    <t>JinZu-App client authentication-Test-3</t>
+  </si>
+  <si>
+    <t>good request, correct OAuth2.0,data retrieved</t>
+  </si>
+  <si>
+    <t>bad request, wrong clientId/clientSecret</t>
+  </si>
+  <si>
+    <t>bad request,No Auth</t>
+  </si>
+  <si>
+    <t>tybk</t>
+  </si>
+  <si>
+    <t>b10d0439-07e2-4dc0-9a2d-2fd33a9e399d</t>
+  </si>
+  <si>
+    <t>JinZu-App client authentication-Test-4</t>
+  </si>
+  <si>
+    <t>JinZu-App client authentication-Test-5</t>
+  </si>
+  <si>
+    <t>JinZu-App client authentication-Test-6</t>
+  </si>
+  <si>
+    <t>good request,No Auth</t>
+  </si>
+  <si>
+    <t>good request, different clientId/clientSecret</t>
+  </si>
 </sst>
 </file>
 
@@ -895,7 +960,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -906,6 +971,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,15 +1256,15 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" style="1"/>
-    <col min="4" max="4" width="36.54296875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="12.54296875" style="1"/>
+    <col min="1" max="2" width="30.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" style="1"/>
+    <col min="4" max="4" width="36.5546875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="12.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1484,19 +1550,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D13" sqref="D1:D1048576"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="90.7265625" style="6" customWidth="1"/>
-    <col min="4" max="6" width="12.54296875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="2" width="30.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="90.77734375" style="6" customWidth="1"/>
+    <col min="4" max="6" width="12.5546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1516,7 +1582,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -1536,7 +1602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
@@ -1556,7 +1622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -1576,7 +1642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -1596,7 +1662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
@@ -1616,7 +1682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
@@ -1636,7 +1702,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>48</v>
       </c>
@@ -1656,7 +1722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -1676,7 +1742,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
@@ -1696,7 +1762,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
@@ -1716,7 +1782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>55</v>
       </c>
@@ -1736,7 +1802,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1756,7 +1822,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>61</v>
       </c>
@@ -1816,7 +1882,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>63</v>
       </c>
@@ -1856,7 +1922,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>68</v>
       </c>
@@ -1876,7 +1942,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>70</v>
       </c>
@@ -1916,7 +1982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
@@ -1936,7 +2002,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>77</v>
       </c>
@@ -1956,7 +2022,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>82</v>
       </c>
@@ -1996,7 +2062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>84</v>
       </c>
@@ -2016,7 +2082,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>85</v>
       </c>
@@ -2036,7 +2102,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>91</v>
       </c>
@@ -2056,7 +2122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>92</v>
       </c>
@@ -2076,7 +2142,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="13.05" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>93</v>
       </c>
@@ -2351,15 +2417,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="40.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-    <col min="6" max="7" width="12.6328125" customWidth="1"/>
+    <col min="1" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2382,7 +2448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -2419,15 +2485,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="40.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-    <col min="6" max="7" width="12.6328125" customWidth="1"/>
+    <col min="1" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2450,7 +2516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>122</v>
       </c>
@@ -2487,15 +2553,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="40.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-    <col min="6" max="7" width="12.6328125" customWidth="1"/>
+    <col min="1" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2518,7 +2584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>123</v>
       </c>
@@ -2551,19 +2617,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FACB25C-715F-46EA-8323-1EF68080F322}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="40.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-    <col min="6" max="7" width="12.6328125" customWidth="1"/>
+    <col min="1" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2586,7 +2652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>126</v>
       </c>
@@ -2620,18 +2686,18 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" customWidth="1"/>
-    <col min="3" max="3" width="40.6328125" customWidth="1"/>
-    <col min="4" max="4" width="20.6328125" customWidth="1"/>
-    <col min="6" max="7" width="12.6328125" customWidth="1"/>
+    <col min="1" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="6" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2654,7 +2720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>128</v>
       </c>
@@ -2681,4 +2747,224 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9467BD-153D-41EA-A440-BE3AFBA58084}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" s="8">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8">
+        <v>403</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59ED7702-9547-4AEE-82DC-811C1B12C606}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G2" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" s="3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="3">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add cache controler case of jinzu api-engine
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FEF183-C67E-40C1-9BAB-19A41F21A00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E25796-9869-4AE6-84DF-53FE9C25D7D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="636" yWindow="588" windowWidth="21960" windowHeight="12408" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="getSiteDetails" sheetId="9" r:id="rId8"/>
     <sheet name="getSchemaWithAuth" sheetId="10" r:id="rId9"/>
     <sheet name="getAllCacheStatsWithAuth" sheetId="11" r:id="rId10"/>
+    <sheet name="getAllCacheNames" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="159">
   <si>
     <t>description</t>
   </si>
@@ -893,35 +894,61 @@
   <si>
     <t>good request, different clientId/clientSecret</t>
   </si>
+  <si>
+    <t>Operate success.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[
+    "subscriptionCache",
+    "entityDataCache",
+    "graphQLSchemaCache",
+    "kgCache",
+    "connectorMetaDataCache"
+  ]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>get all cache names</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JinZu-ApiEngine-CacheController-Test-1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>rspData</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1267,7 +1294,7 @@
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" style="1"/>
@@ -1275,7 +1302,7 @@
     <col min="5" max="16384" width="12.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1301,7 +1328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -1323,7 +1350,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
@@ -1347,7 +1374,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -1371,7 +1398,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -1393,7 +1420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -1415,7 +1442,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -1437,7 +1464,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>1</v>
@@ -1459,7 +1486,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>1</v>
@@ -1481,7 +1508,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>1</v>
@@ -1503,7 +1530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>1</v>
@@ -1525,7 +1552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
         <v>1</v>
@@ -1558,11 +1585,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59ED7702-9547-4AEE-82DC-811C1B12C606}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
@@ -1573,7 +1600,7 @@
     <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1596,7 +1623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>149</v>
       </c>
@@ -1619,7 +1646,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>150</v>
       </c>
@@ -1642,7 +1669,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>151</v>
       </c>
@@ -1659,6 +1686,69 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D302976-6940-4270-B1B7-132C4D0E2581}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="58.21875" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="3">
+        <v>200</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1672,7 +1762,7 @@
       <selection activeCell="A2" sqref="A1:F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="90.77734375" style="6" customWidth="1"/>
@@ -1680,7 +1770,7 @@
     <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1700,7 +1790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -1720,7 +1810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
@@ -1740,7 +1830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.05" customHeight="1">
+    <row r="4" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -1760,7 +1850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.05" customHeight="1">
+    <row r="5" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -1780,7 +1870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
@@ -1800,7 +1890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
@@ -1820,7 +1910,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>48</v>
       </c>
@@ -1840,7 +1930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -1860,7 +1950,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
@@ -1880,7 +1970,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
@@ -1900,7 +1990,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>55</v>
       </c>
@@ -1920,7 +2010,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
@@ -1940,7 +2030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>61</v>
       </c>
@@ -1960,7 +2050,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>62</v>
       </c>
@@ -1980,7 +2070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>62</v>
       </c>
@@ -2000,7 +2090,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>63</v>
       </c>
@@ -2020,7 +2110,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>64</v>
       </c>
@@ -2040,7 +2130,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>68</v>
       </c>
@@ -2060,7 +2150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>70</v>
       </c>
@@ -2080,7 +2170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>74</v>
       </c>
@@ -2100,7 +2190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
@@ -2120,7 +2210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>77</v>
       </c>
@@ -2140,7 +2230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>82</v>
       </c>
@@ -2160,7 +2250,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>83</v>
       </c>
@@ -2180,7 +2270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>84</v>
       </c>
@@ -2200,7 +2290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>85</v>
       </c>
@@ -2220,7 +2310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>91</v>
       </c>
@@ -2240,7 +2330,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>92</v>
       </c>
@@ -2260,7 +2350,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>93</v>
       </c>
@@ -2280,7 +2370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>94</v>
       </c>
@@ -2300,7 +2390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>95</v>
       </c>
@@ -2320,7 +2410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>96</v>
       </c>
@@ -2340,7 +2430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>99</v>
       </c>
@@ -2360,7 +2450,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>100</v>
       </c>
@@ -2380,7 +2470,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>101</v>
       </c>
@@ -2400,7 +2490,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>102</v>
       </c>
@@ -2420,7 +2510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>103</v>
       </c>
@@ -2440,7 +2530,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>104</v>
       </c>
@@ -2460,7 +2550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>107</v>
       </c>
@@ -2480,7 +2570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>108</v>
       </c>
@@ -2500,7 +2590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>109</v>
       </c>
@@ -2535,13 +2625,13 @@
       <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="110.44140625" customWidth="1"/>
     <col min="16" max="16" width="51.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -2570,7 +2660,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -2599,7 +2689,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
@@ -2628,7 +2718,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="409.6">
+    <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -2657,7 +2747,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="409.6">
+    <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
@@ -2686,7 +2776,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>46</v>
       </c>
@@ -2715,7 +2805,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
@@ -2744,7 +2834,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>48</v>
       </c>
@@ -2773,7 +2863,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>54</v>
       </c>
@@ -2802,7 +2892,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
@@ -2831,7 +2921,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
@@ -2860,7 +2950,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>55</v>
       </c>
@@ -2889,7 +2979,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
@@ -2918,7 +3008,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>61</v>
       </c>
@@ -2947,7 +3037,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>62</v>
       </c>
@@ -2976,7 +3066,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>62</v>
       </c>
@@ -3005,7 +3095,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>63</v>
       </c>
@@ -3034,7 +3124,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>64</v>
       </c>
@@ -3063,7 +3153,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>68</v>
       </c>
@@ -3092,7 +3182,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>70</v>
       </c>
@@ -3121,7 +3211,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>74</v>
       </c>
@@ -3150,7 +3240,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>75</v>
       </c>
@@ -3179,7 +3269,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>77</v>
       </c>
@@ -3208,7 +3298,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>82</v>
       </c>
@@ -3237,7 +3327,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>83</v>
       </c>
@@ -3266,7 +3356,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>84</v>
       </c>
@@ -3295,7 +3385,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>85</v>
       </c>
@@ -3324,7 +3414,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>91</v>
       </c>
@@ -3353,7 +3443,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>92</v>
       </c>
@@ -3382,7 +3472,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>93</v>
       </c>
@@ -3411,7 +3501,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>94</v>
       </c>
@@ -3440,7 +3530,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>95</v>
       </c>
@@ -3469,7 +3559,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>96</v>
       </c>
@@ -3498,7 +3588,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>99</v>
       </c>
@@ -3527,7 +3617,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>100</v>
       </c>
@@ -3556,7 +3646,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>101</v>
       </c>
@@ -3585,7 +3675,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>102</v>
       </c>
@@ -3614,7 +3704,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>103</v>
       </c>
@@ -3643,7 +3733,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>104</v>
       </c>
@@ -3672,7 +3762,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>107</v>
       </c>
@@ -3701,7 +3791,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>108</v>
       </c>
@@ -3730,7 +3820,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>109</v>
       </c>
@@ -3774,7 +3864,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.05" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" customWidth="1"/>
@@ -3782,7 +3872,7 @@
     <col min="6" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.05" customHeight="1">
+    <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3805,7 +3895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.05" customHeight="1">
+    <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -3843,7 +3933,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.05" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" customWidth="1"/>
@@ -3851,7 +3941,7 @@
     <col min="6" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.05" customHeight="1">
+    <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3874,7 +3964,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.05" customHeight="1">
+    <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>122</v>
       </c>
@@ -3912,7 +4002,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.05" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" customWidth="1"/>
@@ -3920,7 +4010,7 @@
     <col min="6" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.05" customHeight="1">
+    <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3943,7 +4033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.05" customHeight="1">
+    <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>123</v>
       </c>
@@ -3981,7 +4071,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.05" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" customWidth="1"/>
@@ -3989,7 +4079,7 @@
     <col min="6" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.05" customHeight="1">
+    <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4012,7 +4102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.05" customHeight="1">
+    <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>126</v>
       </c>
@@ -4050,7 +4140,7 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.05" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" customWidth="1"/>
@@ -4058,7 +4148,7 @@
     <col min="6" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.05" customHeight="1">
+    <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4081,7 +4171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.05" customHeight="1">
+    <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>128</v>
       </c>
@@ -4119,7 +4209,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.44140625" bestFit="1" customWidth="1"/>
@@ -4130,7 +4220,7 @@
     <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -4153,7 +4243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>141</v>
       </c>
@@ -4176,7 +4266,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>142</v>
       </c>
@@ -4199,7 +4289,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>143</v>
       </c>

</xml_diff>

<commit_message>
update test case of jinzu
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494A71FE-4DBC-478D-8D64-3E17C44B3DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D0EB55-F813-474A-8FF5-93111CA11813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1764" yWindow="2808" windowWidth="21960" windowHeight="12408" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="163">
   <si>
     <t>description</t>
   </si>
@@ -396,57 +396,7 @@
     <t>queryString</t>
   </si>
   <si>
-    <t>JasonModelSchemaForLeaseDetails.JSON</t>
-  </si>
-  <si>
     <t>JasonModelSchemaForLeaseList.JSON</t>
-  </si>
-  <si>
-    <t>{Lease(cond:"{project:{_eq:99}}", order:"") {
-	lease_type_gb
-	lending
-	lposition
-	invoice_no
-	project
-	lease_type_yj
-	brand_name
-	unit_price
-	serial_num
-	discount_ratio
-	transfer_price
-	lease_net_val
-	nominal_cost
-	supplier
-	asset_type
-	name
-	lease_type
-	position
-	id
-	purchase_time
-	status
-	lease_group
-	product_model
-	Refer_To_Power_Station(cond:"", order:"") {
-		id
-		Compose_Of_Site(cond:"", order:"") {
-			avg_annual_eq_hours
-			avg_irradiance
-			capacity
-			city
-			commissioning_date
-			grid_inject_production
-			id
-			irradiance
-			location
-			name
-			power_station
-			state
-			sys_engaged_date
-			type
-			voltage_degree
-		}
-	}
-}}</t>
   </si>
   <si>
     <t>根据project id获取租赁物信息列表</t>
@@ -950,6 +900,54 @@
 	"connectorMetaDataCache",
 	"kgCache"
 ]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{Lease(cond:"{project:{_eq:99}}", order:"") {
+	lease_type_gb
+	lending
+	lposition
+	invoice_no
+	project
+	lease_type_yj
+	brand_name
+	unit_price
+	serial_num
+	discount_ratio
+	transfer_price
+	lease_net_val
+	nominal_cost
+	supplier
+	asset_type
+	name
+	lease_type
+	position
+	id
+	purchase_time
+	status
+	lease_group
+	product_model
+	Refer_To_Power_Station(cond:"", order:"") {
+		id
+		Compose_Of_Site(cond:"", order:"") {
+			avg_annual_eq_hours
+			avg_irradiance
+			capacity
+			city
+			commissioning_date
+			grid_inject_production
+			id
+			irradiance
+			location
+			name
+			power_station
+			state
+			sys_engaged_date
+			type
+			voltage_degree
+		}
+	}
+}}</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1640,16 +1638,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -1657,22 +1655,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>140</v>
       </c>
       <c r="G2" s="3">
         <v>200</v>
@@ -1680,22 +1678,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G3" s="3">
         <v>200</v>
@@ -1703,10 +1701,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1727,7 +1725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D302976-6940-4270-B1B7-132C4D0E2581}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1747,7 +1745,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -1761,13 +1759,13 @@
     </row>
     <row r="2" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D2" s="3">
         <v>200</v>
@@ -1776,7 +1774,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1809,10 +1807,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -1826,16 +1824,16 @@
     </row>
     <row r="2" spans="1:7" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>158</v>
       </c>
       <c r="E2" s="3">
         <v>200</v>
@@ -1844,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2751,13 +2749,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2780,13 +2778,13 @@
         <v>9</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2809,13 +2807,13 @@
         <v>9</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.25">
@@ -2838,13 +2836,13 @@
         <v>9</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.25">
@@ -2867,13 +2865,13 @@
         <v>9</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H5" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2896,13 +2894,13 @@
         <v>9</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H6" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2925,13 +2923,13 @@
         <v>9</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H7" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2954,13 +2952,13 @@
         <v>9</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H8" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2983,13 +2981,13 @@
         <v>51</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H9" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I9" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -3012,13 +3010,13 @@
         <v>19</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H10" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I10" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -3041,13 +3039,13 @@
         <v>23</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H11" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I11" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3070,13 +3068,13 @@
         <v>59</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H12" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -3099,13 +3097,13 @@
         <v>9</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H13" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3128,13 +3126,13 @@
         <v>9</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H14" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3157,13 +3155,13 @@
         <v>9</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H15" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3186,13 +3184,13 @@
         <v>9</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H16" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3215,13 +3213,13 @@
         <v>9</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H17" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I17" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3244,13 +3242,13 @@
         <v>66</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H18" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3273,13 +3271,13 @@
         <v>9</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H19" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3302,13 +3300,13 @@
         <v>9</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H20" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3331,13 +3329,13 @@
         <v>9</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H21" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I21" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3360,13 +3358,13 @@
         <v>9</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H22" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3389,13 +3387,13 @@
         <v>9</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H23" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I23" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3418,13 +3416,13 @@
         <v>9</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H24" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3447,13 +3445,13 @@
         <v>9</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H25" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3476,13 +3474,13 @@
         <v>9</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H26" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I26" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3505,13 +3503,13 @@
         <v>9</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H27" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I27" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -3534,13 +3532,13 @@
         <v>9</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H28" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I28" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3563,13 +3561,13 @@
         <v>9</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H29" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I29" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3592,13 +3590,13 @@
         <v>9</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H30" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I30" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3621,13 +3619,13 @@
         <v>9</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H31" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I31" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3650,13 +3648,13 @@
         <v>9</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H32" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I32" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3679,13 +3677,13 @@
         <v>9</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H33" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I33" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3708,13 +3706,13 @@
         <v>9</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H34" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I34" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3737,13 +3735,13 @@
         <v>9</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H35" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I35" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3766,13 +3764,13 @@
         <v>9</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H36" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I36" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3795,13 +3793,13 @@
         <v>9</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H37" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I37" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3824,13 +3822,13 @@
         <v>9</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H38" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I38" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3853,13 +3851,13 @@
         <v>9</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H39" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I39" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I39" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3882,13 +3880,13 @@
         <v>9</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H40" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I40" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3911,13 +3909,13 @@
         <v>9</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H41" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I41" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I41" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3940,13 +3938,13 @@
         <v>9</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H42" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I42" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="I42" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -3958,21 +3956,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52831BC6-0353-44A5-AF16-53FEEB981D2D}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="6" max="7" width="12.6640625" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -3983,19 +3980,16 @@
         <v>118</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>116</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>117</v>
       </c>
@@ -4003,18 +3997,15 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>119</v>
+        <v>129</v>
+      </c>
+      <c r="D2" s="3">
+        <v>200</v>
       </c>
       <c r="E2" s="3">
-        <v>200</v>
-      </c>
-      <c r="F2" s="3">
-        <v>100000</v>
-      </c>
-      <c r="G2" s="3" t="s">
+        <v>100000</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4030,14 +4021,14 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="30.6640625" customWidth="1"/>
     <col min="3" max="3" width="40.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
     <col min="6" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4066,16 +4057,16 @@
     </row>
     <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" s="3">
         <v>200</v>
@@ -4135,16 +4126,16 @@
     </row>
     <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E2" s="3">
         <v>200</v>
@@ -4204,16 +4195,16 @@
     </row>
     <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E2" s="3">
         <v>200</v>
@@ -4273,16 +4264,16 @@
     </row>
     <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>130</v>
       </c>
       <c r="E2" s="3">
         <v>200</v>
@@ -4328,16 +4319,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>136</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
@@ -4345,22 +4336,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>140</v>
       </c>
       <c r="G2" s="3">
         <v>200</v>
@@ -4368,22 +4359,22 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>147</v>
-      </c>
       <c r="D3" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G3" s="8">
         <v>403</v>
@@ -4391,10 +4382,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>

</xml_diff>

<commit_message>
update case of apiengine
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D0EB55-F813-474A-8FF5-93111CA11813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C388996-EB85-4C07-A834-82FA670C965B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="164">
   <si>
     <t>description</t>
   </si>
@@ -949,6 +949,10 @@
 	}
 }}</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connector execution fail with code: 106602 exception</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1856,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:F42"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2105,7 +2109,7 @@
         <v>101403</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>59</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3958,7 +3962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52831BC6-0353-44A5-AF16-53FEEB981D2D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add licenseConfigEncrypted on cacheConfig update result of case
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8DD5DD-89EB-49FF-8C33-254452F6D99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF808FBB-C72F-47B7-994F-9093C2A64236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -893,16 +893,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>[
-	"entityDataCache",
-	"subscriptionCache",
-	"graphQLSchemaCache",
-	"connectorMetaDataCache",
-	"kgCache"
-]</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>{Lease(cond:"{project:{_eq:99}}", order:"") {
 	lease_type_gb
 	lending
@@ -948,6 +938,17 @@
 		}
 	}
 }}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[
+	"entityDataCache",
+	"subscriptionCache",
+	"licenseConfigEncrypted",
+	"graphQLSchemaCache",
+	"connectorMetaDataCache",
+	"kgCache"
+]</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1725,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D302976-6940-4270-B1B7-132C4D0E2581}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1757,7 +1758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="105.6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>154</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>153</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D2" s="3">
         <v>200</v>
@@ -1856,7 +1857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE22B0A1-EDF6-487D-8C5B-FE5F049504FE}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
@@ -4043,7 +4044,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
update seach api engine cache result
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
+++ b/src/main/resources/test-data-xls/jinzu-api-engine-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF808FBB-C72F-47B7-994F-9093C2A64236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64FF193-FF7A-4033-81A3-D4343C0F2CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5556" yWindow="3756" windowWidth="17280" windowHeight="10044" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getDataEntities" sheetId="2" r:id="rId1"/>
@@ -943,8 +943,8 @@
   <si>
     <t>[
 	"entityDataCache",
+	"licenseConfigEncrypted",
 	"subscriptionCache",
-	"licenseConfigEncrypted",
 	"graphQLSchemaCache",
 	"connectorMetaDataCache",
 	"kgCache"
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>